<commit_message>
Update chart in Excel
</commit_message>
<xml_diff>
--- a/DATA/CLEAN/merged_data_normalized_CHART.xlsx
+++ b/DATA/CLEAN/merged_data_normalized_CHART.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carinamanitius/Documents/GitHub/Enviro_Impacts_COVID/DATA/CLEAN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{32B11556-D693-5749-98F5-39CD5087B08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4378FA6C-BB31-AE4E-BA77-DA9234DAE361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30260" yWindow="500" windowWidth="38380" windowHeight="21100" xr2:uid="{3DAE8AB0-18CE-D54A-9332-143FC6C592F8}"/>
   </bookViews>
@@ -10526,7 +10526,7 @@
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+      <selection activeCell="U22" sqref="U22:V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add municipal waste and dynamic plotly chart
</commit_message>
<xml_diff>
--- a/DATA/CLEAN/merged_data_normalized_CHART.xlsx
+++ b/DATA/CLEAN/merged_data_normalized_CHART.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carinamanitius/Documents/GitHub/Enviro_Impacts_COVID/DATA/CLEAN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4378FA6C-BB31-AE4E-BA77-DA9234DAE361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07D7A5F-A011-2449-A815-76AF693E6FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30260" yWindow="500" windowWidth="38380" windowHeight="21100" xr2:uid="{3DAE8AB0-18CE-D54A-9332-143FC6C592F8}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Year</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>USA_WFH_share</t>
+  </si>
+  <si>
+    <t>total_municipal_waste_tonnes</t>
   </si>
 </sst>
 </file>
@@ -620,24 +623,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -655,16 +641,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -696,12 +672,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4844,6 +4817,203 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000015-F523-F24B-A8EF-89DAAAA22AA5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="22"/>
+          <c:order val="22"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>merged_data_normalized!$X$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total_municipal_waste_tonnes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>merged_data_normalized!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>merged_data_normalized!$X$2:$X$26</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>89.340892944894804</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.150214427779602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.300308398204606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.125508350569206</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.271632703624206</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.939212838563805</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92.862627968828903</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93.4546484903818</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>92.47155221621</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91.442873783962398</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.790694395584694</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.1527508763957</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.6186320151009</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>91.697476829069601</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>92.357665262699697</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>93.422207134634306</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95.677497334196602</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>96.076786088270595</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99.604270213223202</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>101.08603255907499</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>101.993706103218</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>100.236534441906</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4FF6-744F-B7DC-7A541926DDBE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5263,7 +5433,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000000-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5458,7 +5628,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000001-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5653,7 +5823,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000002-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5848,7 +6018,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000003-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6043,7 +6213,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000004-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6238,7 +6408,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000005-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6435,7 +6605,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000006-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6632,7 +6802,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000007-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6829,7 +6999,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000008-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7026,7 +7196,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000009-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7187,7 +7357,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{0000000A-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7387,7 +7557,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{0000000B-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7558,7 +7728,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{0000000D-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7729,7 +7899,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{0000000E-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7927,7 +8097,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{0000000F-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8083,7 +8253,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000010-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8284,7 +8454,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000011-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000011-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8481,7 +8651,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000012-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8648,7 +8818,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000013-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000013-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8809,7 +8979,204 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000014-4844-8D43-BC1C-AE97D5EBB8A9}"/>
+              <c16:uniqueId val="{00000014-247B-F040-A224-FF3199363B66}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="22"/>
+          <c:order val="20"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>merged_data_normalized!$X$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total_municipal_waste_tonnes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>merged_data_normalized!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>merged_data_normalized!$X$2:$X$26</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>89.340892944894804</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.150214427779602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.300308398204606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.125508350569206</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.271632703624206</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.939212838563805</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92.862627968828903</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93.4546484903818</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>92.47155221621</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91.442873783962398</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.790694395584694</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.1527508763957</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.6186320151009</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>91.697476829069601</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>92.357665262699697</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>93.422207134634306</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95.677497334196602</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>96.076786088270595</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99.604270213223202</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>101.08603255907499</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>101.993706103218</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>100.236534441906</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-247B-F040-A224-FF3199363B66}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10168,22 +10535,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
+      <xdr:colOff>82550</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D8A615-E7ED-BC4F-AD3A-761B814431E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4D266D0-D81A-E24C-A546-8C3E6C8CCDC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10523,15 +10890,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6B569D-1E43-424A-A533-2751E04E35CF}">
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22:V25"/>
+    <sheetView tabSelected="1" topLeftCell="I21" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10601,8 +10968,11 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2000</v>
       </c>
@@ -10650,8 +11020,11 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
+      <c r="X2" s="1">
+        <v>89.340892944894804</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -10703,8 +11076,11 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
+      <c r="X3" s="1">
+        <v>89.150214427779602</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -10756,8 +11132,11 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
+      <c r="X4" s="1">
+        <v>90.300308398204606</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -10811,8 +11190,11 @@
       <c r="W5" s="1">
         <v>42.414905026394003</v>
       </c>
+      <c r="X5" s="1">
+        <v>90.125508350569206</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -10866,8 +11248,11 @@
       <c r="W6" s="1">
         <v>57.298894471852499</v>
       </c>
+      <c r="X6" s="1">
+        <v>91.271632703624206</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -10921,8 +11306,11 @@
       <c r="W7" s="1">
         <v>47.224762811821599</v>
       </c>
+      <c r="X7" s="1">
+        <v>91.939212838563805</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -10976,8 +11364,11 @@
       <c r="W8" s="1">
         <v>48.521480187834499</v>
       </c>
+      <c r="X8" s="1">
+        <v>92.862627968828903</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -11031,8 +11422,11 @@
       <c r="W9" s="1">
         <v>55.928656110658501</v>
       </c>
+      <c r="X9" s="1">
+        <v>93.4546484903818</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -11086,8 +11480,11 @@
       <c r="W10" s="1">
         <v>63.086452025123798</v>
       </c>
+      <c r="X10" s="1">
+        <v>92.47155221621</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -11141,8 +11538,11 @@
       <c r="W11" s="1">
         <v>89.032339700018596</v>
       </c>
+      <c r="X11" s="1">
+        <v>91.442873783962398</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -11206,8 +11606,11 @@
       <c r="W12" s="1">
         <v>74.884103446986103</v>
       </c>
+      <c r="X12" s="1">
+        <v>91.790694395584694</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -11273,8 +11676,11 @@
       <c r="W13" s="1">
         <v>63.821708544227803</v>
       </c>
+      <c r="X13" s="1">
+        <v>92.1527508763957</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -11342,8 +11748,11 @@
       <c r="W14" s="1">
         <v>80.202748050157197</v>
       </c>
+      <c r="X14" s="1">
+        <v>91.6186320151009</v>
+      </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -11413,8 +11822,11 @@
       <c r="W15" s="1">
         <v>75.419610622782301</v>
       </c>
+      <c r="X15" s="1">
+        <v>91.697476829069601</v>
+      </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -11482,8 +11894,11 @@
       <c r="W16" s="1">
         <v>89.684248435595705</v>
       </c>
+      <c r="X16" s="1">
+        <v>92.357665262699697</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -11551,8 +11966,11 @@
       <c r="W17" s="1">
         <v>94.973512645069405</v>
       </c>
+      <c r="X17" s="1">
+        <v>93.422207134634306</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -11620,8 +12038,11 @@
       <c r="W18" s="1">
         <v>82.835176658033802</v>
       </c>
+      <c r="X18" s="1">
+        <v>95.677497334196602</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2017</v>
       </c>
@@ -11691,8 +12112,11 @@
       <c r="W19" s="1">
         <v>96.943499042887098</v>
       </c>
+      <c r="X19" s="1">
+        <v>96.076786088270595</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2018</v>
       </c>
@@ -11762,8 +12186,11 @@
       <c r="W20" s="1">
         <v>73.655686986205595</v>
       </c>
+      <c r="X20" s="1">
+        <v>99.604270213223202</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -11833,8 +12260,11 @@
       <c r="W21" s="1">
         <v>100</v>
       </c>
+      <c r="X21" s="1">
+        <v>100</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2020</v>
       </c>
@@ -11904,8 +12334,11 @@
       <c r="W22" s="1">
         <v>647.86270040780403</v>
       </c>
+      <c r="X22" s="1">
+        <v>101.08603255907499</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2021</v>
       </c>
@@ -11975,8 +12408,11 @@
       <c r="W23" s="1">
         <v>469.57719455662902</v>
       </c>
+      <c r="X23" s="1">
+        <v>101.993706103218</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2022</v>
       </c>
@@ -12044,8 +12480,11 @@
       <c r="W24" s="1">
         <v>424.56398915745399</v>
       </c>
+      <c r="X24" s="1">
+        <v>100.236534441906</v>
+      </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2023</v>
       </c>
@@ -12091,8 +12530,9 @@
       <c r="W25" s="1">
         <v>402.49723790743201</v>
       </c>
+      <c r="X25" s="1"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2024</v>
       </c>
@@ -12122,27 +12562,28 @@
       <c r="W26" s="1">
         <v>386.81093599381501</v>
       </c>
+      <c r="X26" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B23:W26">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+  <conditionalFormatting sqref="B22:W26">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
+      <formula>LEN(TRIM(B22))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
-      <formula>LEN(TRIM(B23))=0</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:W22">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B22))=0</formula>
+  <conditionalFormatting sqref="X22:X26">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(X22))=0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>